<commit_message>
cadastro de usuarios concluido
</commit_message>
<xml_diff>
--- a/_adm/_Cadastros app MYSQL.xlsx
+++ b/_adm/_Cadastros app MYSQL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\securedb\_adm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4EBF70B-CB0D-4F7E-AFFF-046FBC7F0852}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D718325F-4F8B-40AA-AFF4-8687A07917C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A00387D4-E64E-4392-9601-70E56E667E9A}"/>
   </bookViews>
@@ -20,6 +20,7 @@
     <sheet name="Viewer" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -560,9 +561,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -576,6 +574,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -583,95 +584,509 @@
   </cellStyles>
   <dxfs count="93">
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -1067,558 +1482,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -1938,6 +1801,81 @@
         <family val="3"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1998,7 +1936,70 @@
         <family val="3"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2014,198 +2015,198 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{CE6B4342-CBFA-473D-8302-1E748C465A67}" name="Tabela10" displayName="Tabela10" ref="B4:G8" totalsRowShown="0" dataDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{CE6B4342-CBFA-473D-8302-1E748C465A67}" name="Tabela10" displayName="Tabela10" ref="B4:G8" totalsRowShown="0" dataDxfId="92">
   <autoFilter ref="B4:G8" xr:uid="{EA0BA91C-0053-4873-B377-F4C9B118EF81}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{4312BCB8-21CE-427F-88A7-93C626B67CB4}" name="idcia" dataDxfId="43"/>
-    <tableColumn id="2" xr3:uid="{CF3C2B84-D621-45A1-B55F-0A0AA8694AFF}" name="cianame" dataDxfId="42"/>
-    <tableColumn id="5" xr3:uid="{11AC588F-E33E-498E-90C3-DA4FAB1B095C}" name="respname" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{6C76FE8B-145E-4E8B-82FE-4FBA8DBA606A}" name="email" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{BEE80F0E-A884-4CEE-8FED-72BF33FFC95A}" name="celphone" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{BB764F07-0EF8-4779-AAF3-081A310C3134}" name="status" dataDxfId="41"/>
+    <tableColumn id="1" xr3:uid="{4312BCB8-21CE-427F-88A7-93C626B67CB4}" name="idcia" dataDxfId="91"/>
+    <tableColumn id="2" xr3:uid="{CF3C2B84-D621-45A1-B55F-0A0AA8694AFF}" name="cianame" dataDxfId="90"/>
+    <tableColumn id="5" xr3:uid="{11AC588F-E33E-498E-90C3-DA4FAB1B095C}" name="respname" dataDxfId="89"/>
+    <tableColumn id="6" xr3:uid="{6C76FE8B-145E-4E8B-82FE-4FBA8DBA606A}" name="email" dataDxfId="88"/>
+    <tableColumn id="7" xr3:uid="{BEE80F0E-A884-4CEE-8FED-72BF33FFC95A}" name="celphone" dataDxfId="87"/>
+    <tableColumn id="3" xr3:uid="{BB764F07-0EF8-4779-AAF3-081A310C3134}" name="status" dataDxfId="86"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium25" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{117599F9-7BC4-4FFC-A14F-9880FA008D62}" name="Tabela4" displayName="Tabela4" ref="C3:C8" totalsRowShown="0" headerRowDxfId="84" dataDxfId="83" tableBorderDxfId="82">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{117599F9-7BC4-4FFC-A14F-9880FA008D62}" name="Tabela4" displayName="Tabela4" ref="C3:C8" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39" tableBorderDxfId="38">
   <autoFilter ref="C3:C8" xr:uid="{C6E10A1E-B17D-4DA0-A721-41F80C7BCC6E}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{FEFBDF3E-6414-4FDF-8922-F1B23A103788}" name="TNS" dataDxfId="81"/>
+    <tableColumn id="1" xr3:uid="{FEFBDF3E-6414-4FDF-8922-F1B23A103788}" name="TNS" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium24" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{2CB9C6E2-B2BE-4447-A442-E97A818F5177}" name="Tabela414" displayName="Tabela414" ref="F3:F8" totalsRowShown="0" headerRowDxfId="80" dataDxfId="79" tableBorderDxfId="78">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{2CB9C6E2-B2BE-4447-A442-E97A818F5177}" name="Tabela414" displayName="Tabela414" ref="F3:F8" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35" tableBorderDxfId="34">
   <autoFilter ref="F3:F8" xr:uid="{5D526376-D6EB-4486-89BA-AEDFFE8888E9}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{B4A2BFFC-74D7-482D-9CB6-444A21A14746}" name="PROGRAM" dataDxfId="77"/>
+    <tableColumn id="1" xr3:uid="{B4A2BFFC-74D7-482D-9CB6-444A21A14746}" name="PROGRAM" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium25" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{1886F047-E801-4F28-9BAE-1E0CDCFFC04D}" name="Tabela115" displayName="Tabela115" ref="F11:I12" totalsRowShown="0" headerRowDxfId="76" dataDxfId="75">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{1886F047-E801-4F28-9BAE-1E0CDCFFC04D}" name="Tabela115" displayName="Tabela115" ref="F11:I12" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
   <autoFilter ref="F11:I12" xr:uid="{5D25EB8E-91DF-4172-B5F4-E533114D351A}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{17FE0A75-2457-40A1-99E9-0A466CC1D9FB}" name="Data" dataDxfId="74"/>
-    <tableColumn id="2" xr3:uid="{B8DF1968-D98D-42A1-8F9B-8A42BB6F4E26}" name="USERNAME" dataDxfId="73"/>
-    <tableColumn id="3" xr3:uid="{CB4BDD2E-CDB2-4077-B902-9D6D8A357D83}" name="OSUSER" dataDxfId="72"/>
-    <tableColumn id="4" xr3:uid="{1466B965-A111-47F5-8CF6-1B6A0F27002E}" name="MACHINE" dataDxfId="71"/>
+    <tableColumn id="1" xr3:uid="{17FE0A75-2457-40A1-99E9-0A466CC1D9FB}" name="Data" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{B8DF1968-D98D-42A1-8F9B-8A42BB6F4E26}" name="USERNAME" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{CB4BDD2E-CDB2-4077-B902-9D6D8A357D83}" name="OSUSER" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{1466B965-A111-47F5-8CF6-1B6A0F27002E}" name="MACHINE" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium25" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{44884F21-7769-4BD2-909A-1E31250F9095}" name="Tabela510" displayName="Tabela510" ref="B6:G13" totalsRowShown="0" headerRowDxfId="70" dataDxfId="69">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{44884F21-7769-4BD2-909A-1E31250F9095}" name="Tabela510" displayName="Tabela510" ref="B6:G13" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <autoFilter ref="B6:G13" xr:uid="{94A45C83-F8A5-4D97-83AD-DA40AE6781D1}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{700AC22E-D27F-4BC7-B7F5-34F1B2137640}" name="QTD" dataDxfId="68"/>
-    <tableColumn id="2" xr3:uid="{A662147F-3BCD-4BDE-AE8D-4149CCCBC801}" name="Username" dataDxfId="67"/>
-    <tableColumn id="3" xr3:uid="{9B37164F-A883-4C40-81DB-B40062874D74}" name="OSUser" dataDxfId="66"/>
-    <tableColumn id="4" xr3:uid="{384C905F-C0E0-4ED0-8095-EEC1CBAB51CA}" name="Machine" dataDxfId="65"/>
-    <tableColumn id="5" xr3:uid="{63466D1C-3057-40D4-93AA-E5F7642EC14D}" name="Program" dataDxfId="64"/>
-    <tableColumn id="6" xr3:uid="{C60D9824-F037-4E66-8F44-2D9C74CC5BCA}" name="Status" dataDxfId="63"/>
+    <tableColumn id="1" xr3:uid="{700AC22E-D27F-4BC7-B7F5-34F1B2137640}" name="QTD" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{A662147F-3BCD-4BDE-AE8D-4149CCCBC801}" name="Username" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{9B37164F-A883-4C40-81DB-B40062874D74}" name="OSUser" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{384C905F-C0E0-4ED0-8095-EEC1CBAB51CA}" name="Machine" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{63466D1C-3057-40D4-93AA-E5F7642EC14D}" name="Program" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{C60D9824-F037-4E66-8F44-2D9C74CC5BCA}" name="Status" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium25" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{0811E8F2-F425-47CB-BCC2-633474B4D7B6}" name="Tabela15" displayName="Tabela15" ref="I6:I7" insertRow="1" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{0811E8F2-F425-47CB-BCC2-633474B4D7B6}" name="Tabela15" displayName="Tabela15" ref="I6:I7" insertRow="1" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <autoFilter ref="I6:I7" xr:uid="{4F731ABB-2DCB-4CA1-97B4-809D15751A10}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{012C9BAF-DECD-45CC-84B2-0007FDA9CD42}" name="USERNAME" dataDxfId="60"/>
+    <tableColumn id="1" xr3:uid="{012C9BAF-DECD-45CC-84B2-0007FDA9CD42}" name="USERNAME" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium25" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{F2FEDA15-E48A-46B2-ADE2-857CC1107CAA}" name="Tabela541113" displayName="Tabela541113" ref="B5:O12" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{F2FEDA15-E48A-46B2-ADE2-857CC1107CAA}" name="Tabela541113" displayName="Tabela541113" ref="B5:O12" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="B5:O12" xr:uid="{FA9BC69B-F4B4-484A-AE2F-15EEF07BADAB}"/>
   <tableColumns count="14">
-    <tableColumn id="2" xr3:uid="{6949D402-5241-4165-95FE-277FA407A798}" name="Username" dataDxfId="57"/>
-    <tableColumn id="3" xr3:uid="{6D86510B-85D5-4AD8-953B-45A251A095FD}" name="OSUser" dataDxfId="56"/>
-    <tableColumn id="4" xr3:uid="{B43A5AAA-6EC3-4D3D-84FA-A51F98E151B8}" name="Machine" dataDxfId="55"/>
-    <tableColumn id="5" xr3:uid="{443BB74C-6BB5-499E-8C22-EFE1D0453E8B}" name="Dt.Inicio" dataDxfId="54"/>
-    <tableColumn id="6" xr3:uid="{F39BB5B0-A3A8-42D2-96E3-7E96DCA65153}" name="Dt.Fim" dataDxfId="53"/>
-    <tableColumn id="1" xr3:uid="{2E5364E9-E283-4547-9F83-61A8050FD41A}" name="Tools" dataDxfId="52"/>
-    <tableColumn id="11" xr3:uid="{1FA6C5E4-E58E-421F-A761-3C635C7DADE4}" name="Sessões por Usuário" dataDxfId="51"/>
-    <tableColumn id="7" xr3:uid="{2AF58C69-2939-48B7-A278-50800C8AFFE3}" name="LogUser" dataDxfId="50"/>
-    <tableColumn id="8" xr3:uid="{5B1FF714-5F0C-4FAA-9E1C-39B57C01928A}" name="Trace" dataDxfId="49"/>
-    <tableColumn id="9" xr3:uid="{E54A7B0F-B61C-4127-8E4C-73E6B24108AB}" name="Cursor Sharing" dataDxfId="48"/>
-    <tableColumn id="10" xr3:uid="{755A179F-FC51-40ED-9A5F-3F57754D6D3E}" name="INIT PL/SQL" dataDxfId="47"/>
-    <tableColumn id="12" xr3:uid="{981E64EF-623C-44A3-816D-E1D80C5EB0BC}" name="OBS" dataDxfId="46"/>
-    <tableColumn id="13" xr3:uid="{BFC22A29-29BA-476F-AF19-4DB9198B27E7}" name="Grantor Username" dataDxfId="45"/>
-    <tableColumn id="14" xr3:uid="{EE723761-82B5-4C7F-9F41-A78AAD6F6D48}" name="Grantor OSUSER" dataDxfId="44"/>
+    <tableColumn id="2" xr3:uid="{6949D402-5241-4165-95FE-277FA407A798}" name="Username" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{6D86510B-85D5-4AD8-953B-45A251A095FD}" name="OSUser" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{B43A5AAA-6EC3-4D3D-84FA-A51F98E151B8}" name="Machine" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{443BB74C-6BB5-499E-8C22-EFE1D0453E8B}" name="Dt.Inicio" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{F39BB5B0-A3A8-42D2-96E3-7E96DCA65153}" name="Dt.Fim" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{2E5364E9-E283-4547-9F83-61A8050FD41A}" name="Tools" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{1FA6C5E4-E58E-421F-A761-3C635C7DADE4}" name="Sessões por Usuário" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{2AF58C69-2939-48B7-A278-50800C8AFFE3}" name="LogUser" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{5B1FF714-5F0C-4FAA-9E1C-39B57C01928A}" name="Trace" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{E54A7B0F-B61C-4127-8E4C-73E6B24108AB}" name="Cursor Sharing" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{755A179F-FC51-40ED-9A5F-3F57754D6D3E}" name="INIT PL/SQL" dataDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{981E64EF-623C-44A3-816D-E1D80C5EB0BC}" name="OBS" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{BFC22A29-29BA-476F-AF19-4DB9198B27E7}" name="Grantor Username" dataDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{EE723761-82B5-4C7F-9F41-A78AAD6F6D48}" name="Grantor OSUSER" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium25" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{6D809C67-C871-4059-9A1D-F2E218B00897}" name="Tabela11" displayName="Tabela11" ref="B11:K14" totalsRowShown="0" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{6D809C67-C871-4059-9A1D-F2E218B00897}" name="Tabela11" displayName="Tabela11" ref="B11:K14" totalsRowShown="0" dataDxfId="85">
   <autoFilter ref="B11:K14" xr:uid="{5C835B22-5BC8-4F39-A059-93F7A987AFB8}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{9E148F98-1FD3-49C1-A9BB-F1A1805EA7F5}" name="iduser" dataDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{1D7712DB-DB75-4B66-8A5E-0AB98D15D1B0}" name="idcia" dataDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{2FAB6B79-A789-4A77-89F6-BA0C56C86D35}" name="name" dataDxfId="37"/>
+    <tableColumn id="1" xr3:uid="{9E148F98-1FD3-49C1-A9BB-F1A1805EA7F5}" name="iduser" dataDxfId="84"/>
+    <tableColumn id="2" xr3:uid="{1D7712DB-DB75-4B66-8A5E-0AB98D15D1B0}" name="idcia" dataDxfId="83"/>
+    <tableColumn id="3" xr3:uid="{2FAB6B79-A789-4A77-89F6-BA0C56C86D35}" name="name" dataDxfId="82"/>
     <tableColumn id="4" xr3:uid="{62787CAB-A3F2-4E0F-A55D-8680E7A300AD}" name="loginuser"/>
     <tableColumn id="5" xr3:uid="{99633B34-30C0-45B9-83B1-67B8F0C06954}" name="Password"/>
-    <tableColumn id="6" xr3:uid="{233A1894-FA95-49D7-AFDC-C98113F737F1}" name="email" dataDxfId="36" dataCellStyle="Hiperlink"/>
-    <tableColumn id="10" xr3:uid="{A5BF7DD2-C44A-4E80-B5E6-E614834AE381}" name="celphone" dataDxfId="3" dataCellStyle="Hiperlink"/>
-    <tableColumn id="7" xr3:uid="{C5E32CB7-6B92-4324-BB4A-D0D7D06693B4}" name="status" dataDxfId="35"/>
-    <tableColumn id="8" xr3:uid="{B2745FC3-C449-4AA1-B9A0-85D0F3464D19}" name="admin" dataDxfId="34"/>
-    <tableColumn id="9" xr3:uid="{7C9F39C1-8A41-45EA-BF5B-F8748B7872C1}" name="superuser" dataDxfId="33"/>
+    <tableColumn id="6" xr3:uid="{233A1894-FA95-49D7-AFDC-C98113F737F1}" name="email" dataDxfId="81" dataCellStyle="Hiperlink"/>
+    <tableColumn id="10" xr3:uid="{A5BF7DD2-C44A-4E80-B5E6-E614834AE381}" name="celphone" dataDxfId="80" dataCellStyle="Hiperlink"/>
+    <tableColumn id="7" xr3:uid="{C5E32CB7-6B92-4324-BB4A-D0D7D06693B4}" name="status" dataDxfId="79"/>
+    <tableColumn id="8" xr3:uid="{B2745FC3-C449-4AA1-B9A0-85D0F3464D19}" name="admin" dataDxfId="78"/>
+    <tableColumn id="9" xr3:uid="{7C9F39C1-8A41-45EA-BF5B-F8748B7872C1}" name="superuser" dataDxfId="77"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium25" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{12B0385F-B1A1-41AC-814A-6522E4A300D7}" name="Tabela117" displayName="Tabela117" ref="B18:D22" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{12B0385F-B1A1-41AC-814A-6522E4A300D7}" name="Tabela117" displayName="Tabela117" ref="B18:D22" totalsRowShown="0" headerRowDxfId="76" dataDxfId="75">
   <autoFilter ref="B18:D22" xr:uid="{4453047C-8941-416A-9E0E-9E5669C82504}"/>
   <tableColumns count="3">
-    <tableColumn id="3" xr3:uid="{79C72FA5-8DE0-4B65-AD54-38A81CB993FA}" name="idcia" dataDxfId="9"/>
-    <tableColumn id="1" xr3:uid="{09C1CEBC-A44B-455A-84FB-54C83A83CA7C}" name="categor" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{86C5BE9C-C7D4-48D0-93C7-7A4D5E54E773}" name="descat" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{79C72FA5-8DE0-4B65-AD54-38A81CB993FA}" name="idcia" dataDxfId="74"/>
+    <tableColumn id="1" xr3:uid="{09C1CEBC-A44B-455A-84FB-54C83A83CA7C}" name="categor" dataDxfId="73"/>
+    <tableColumn id="2" xr3:uid="{86C5BE9C-C7D4-48D0-93C7-7A4D5E54E773}" name="descat" dataDxfId="72"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium25" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{C8030295-3190-4C6E-82FC-477278DBF0E6}" name="Tabela218" displayName="Tabela218" ref="B25:H30" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{C8030295-3190-4C6E-82FC-477278DBF0E6}" name="Tabela218" displayName="Tabela218" ref="B25:H30" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70">
   <autoFilter ref="B25:H30" xr:uid="{74CF12DE-3DF6-45DD-947E-BFE77700D033}"/>
   <tableColumns count="7">
-    <tableColumn id="3" xr3:uid="{D62E88F7-48BD-48B7-BD7F-F18204103C78}" name="idcia" dataDxfId="8"/>
-    <tableColumn id="1" xr3:uid="{92AF37FD-5952-4276-80C0-6A5E7149F8A2}" name="databasename" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{2D00C2D1-6D76-4C1D-A536-B2C399989BEF}" name="category" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{3F93EB93-4C83-4EB3-8C77-D0AC52CC95AC}" name="host" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{D63EAF68-822E-46F9-A1A5-F62C2B2540C8}" name="dbname" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{61D4C29B-D324-4AA3-8F28-C625977E703B}" name="username" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{FD703B5D-208C-4E3D-B57B-DE9584D70A15}" name="password" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{D62E88F7-48BD-48B7-BD7F-F18204103C78}" name="idcia" dataDxfId="69"/>
+    <tableColumn id="1" xr3:uid="{92AF37FD-5952-4276-80C0-6A5E7149F8A2}" name="databasename" dataDxfId="68"/>
+    <tableColumn id="2" xr3:uid="{2D00C2D1-6D76-4C1D-A536-B2C399989BEF}" name="category" dataDxfId="67"/>
+    <tableColumn id="5" xr3:uid="{3F93EB93-4C83-4EB3-8C77-D0AC52CC95AC}" name="host" dataDxfId="66"/>
+    <tableColumn id="6" xr3:uid="{D63EAF68-822E-46F9-A1A5-F62C2B2540C8}" name="dbname" dataDxfId="65"/>
+    <tableColumn id="7" xr3:uid="{61D4C29B-D324-4AA3-8F28-C625977E703B}" name="username" dataDxfId="64"/>
+    <tableColumn id="8" xr3:uid="{FD703B5D-208C-4E3D-B57B-DE9584D70A15}" name="password" dataDxfId="63"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium25" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{009A29F3-4BFA-40BC-81F7-105CE74E7BED}" name="Tabela419" displayName="Tabela419" ref="B34:B39" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" tableBorderDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{009A29F3-4BFA-40BC-81F7-105CE74E7BED}" name="Tabela419" displayName="Tabela419" ref="B34:B39" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61" tableBorderDxfId="60">
   <autoFilter ref="B34:B39" xr:uid="{B229024B-3BC2-4C6D-9586-CC75AE5A0472}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{B43FB459-1AD3-4F77-9D76-578795941534}" name="TNS" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{B43FB459-1AD3-4F77-9D76-578795941534}" name="TNS" dataDxfId="59"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium24" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{65CD7931-A024-4F6D-9967-6CF5AABD86F2}" name="Tabela41420" displayName="Tabela41420" ref="C34:C39" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" tableBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{65CD7931-A024-4F6D-9967-6CF5AABD86F2}" name="Tabela41420" displayName="Tabela41420" ref="C34:C39" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57" tableBorderDxfId="56">
   <autoFilter ref="C34:C39" xr:uid="{E89416BE-A200-4BA3-809B-106F021D56A7}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{ACC89BFB-B9F7-4DB8-A95C-B3FB95412F23}" name="PROGRAM" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{ACC89BFB-B9F7-4DB8-A95C-B3FB95412F23}" name="PROGRAM" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium25" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{8776950F-2CB1-4D74-B675-879D864C7C5A}" name="Tabela11521" displayName="Tabela11521" ref="D34:G35" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{8776950F-2CB1-4D74-B675-879D864C7C5A}" name="Tabela11521" displayName="Tabela11521" ref="D34:G35" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
   <autoFilter ref="D34:G35" xr:uid="{B790A7DD-ED53-4FA8-91ED-16F0C10E4DC1}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{08BA3056-0339-4817-9E3A-B161B0BAE367}" name="Data" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{7A97437C-475E-4C34-B135-DE3B2AD5A7AC}" name="USERNAME" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{332C3A08-2212-40AC-BD5A-B9CE10A33233}" name="OSUSER" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{1C44CCFA-C55A-4A9A-A85D-AB97A44AEFE9}" name="MACHINE" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{08BA3056-0339-4817-9E3A-B161B0BAE367}" name="Data" dataDxfId="52"/>
+    <tableColumn id="2" xr3:uid="{7A97437C-475E-4C34-B135-DE3B2AD5A7AC}" name="USERNAME" dataDxfId="51"/>
+    <tableColumn id="3" xr3:uid="{332C3A08-2212-40AC-BD5A-B9CE10A33233}" name="OSUSER" dataDxfId="50"/>
+    <tableColumn id="4" xr3:uid="{1C44CCFA-C55A-4A9A-A85D-AB97A44AEFE9}" name="MACHINE" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium25" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AE0AF349-CF1A-428A-A441-10B8C64741C7}" name="Tabela1" displayName="Tabela1" ref="C11:D15" totalsRowShown="0" headerRowDxfId="92" dataDxfId="91">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AE0AF349-CF1A-428A-A441-10B8C64741C7}" name="Tabela1" displayName="Tabela1" ref="C11:D15" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
   <autoFilter ref="C11:D15" xr:uid="{FF6AADAE-530D-4CDA-8713-5E777F4D6B64}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{EA1FC018-DD82-49D0-ABC3-079CF18C1AD2}" name="Ambientes" dataDxfId="90"/>
-    <tableColumn id="2" xr3:uid="{F73778B9-D619-4440-81FB-50C8EE9517E0}" name="DESC" dataDxfId="89"/>
+    <tableColumn id="1" xr3:uid="{EA1FC018-DD82-49D0-ABC3-079CF18C1AD2}" name="Ambientes" dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{F73778B9-D619-4440-81FB-50C8EE9517E0}" name="DESC" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium25" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{09D064AD-C27E-4B24-9657-A76B6B8A1E9A}" name="Tabela2" displayName="Tabela2" ref="C18:D23" totalsRowShown="0" headerRowDxfId="88" dataDxfId="87">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{09D064AD-C27E-4B24-9657-A76B6B8A1E9A}" name="Tabela2" displayName="Tabela2" ref="C18:D23" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
   <autoFilter ref="C18:D23" xr:uid="{20F04E8A-D3AC-4A3B-A97F-B3624C6D18AA}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{6567C651-5BD0-43EA-A2D0-5ED018FCFC86}" name="Banco" dataDxfId="86"/>
-    <tableColumn id="2" xr3:uid="{EB59A4AE-D691-4B6E-952B-62CDB1B581FC}" name="Ambiente" dataDxfId="85"/>
+    <tableColumn id="1" xr3:uid="{6567C651-5BD0-43EA-A2D0-5ED018FCFC86}" name="Banco" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{EB59A4AE-D691-4B6E-952B-62CDB1B581FC}" name="Ambiente" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium25" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2510,8 +2511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0080EB5-8FF3-4500-94A4-3766A8BA9D9D}">
   <dimension ref="B3:K39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2521,6 +2522,7 @@
     <col min="5" max="6" width="14.44140625" customWidth="1"/>
     <col min="7" max="7" width="21.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="14.44140625" customWidth="1"/>
+    <col min="11" max="11" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:11" x14ac:dyDescent="0.3">
@@ -2529,7 +2531,7 @@
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>76</v>
       </c>
       <c r="C4" t="s">
@@ -2549,65 +2551,65 @@
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B5" s="15">
+      <c r="B5" s="14">
         <v>1</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15" t="s">
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="15">
+      <c r="B6" s="14">
         <v>2</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15" t="s">
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B7" s="15">
+      <c r="B7" s="14">
         <v>3</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15" t="s">
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B8" s="15">
+      <c r="B8" s="14">
         <v>4</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15" t="s">
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
@@ -2627,7 +2629,7 @@
       <c r="E11" t="s">
         <v>86</v>
       </c>
-      <c r="F11" s="19" t="s">
+      <c r="F11" s="18" t="s">
         <v>99</v>
       </c>
       <c r="G11" t="s">
@@ -2647,75 +2649,75 @@
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B12" s="15">
+      <c r="B12" s="14">
         <v>1</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="14">
         <v>1</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="G12" s="17" t="s">
+      <c r="G12" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="H12" s="17">
+      <c r="H12" s="16">
         <v>11992005722</v>
       </c>
-      <c r="I12" s="15">
+      <c r="I12" s="14">
         <v>1</v>
       </c>
-      <c r="J12" s="15">
+      <c r="J12" s="14">
         <v>1</v>
       </c>
-      <c r="K12" s="15">
+      <c r="K12" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B13" s="15">
+      <c r="B13" s="14">
         <v>2</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="14">
         <v>2</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="G13" s="17" t="s">
+      <c r="G13" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="H13" s="17"/>
-      <c r="I13" s="15">
+      <c r="H13" s="16"/>
+      <c r="I13" s="14">
         <v>1</v>
       </c>
-      <c r="J13" s="15">
+      <c r="J13" s="14">
         <v>1</v>
       </c>
-      <c r="K13" s="15">
+      <c r="K13" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B14" s="15">
+      <c r="B14" s="14">
         <v>3</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="14">
         <v>2</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="15" t="s">
         <v>96</v>
       </c>
       <c r="E14" t="s">
@@ -2724,30 +2726,30 @@
       <c r="F14" t="s">
         <v>101</v>
       </c>
-      <c r="G14" s="17" t="s">
+      <c r="G14" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="H14" s="17"/>
-      <c r="I14" s="15">
+      <c r="H14" s="16"/>
+      <c r="I14" s="14">
         <v>0</v>
       </c>
-      <c r="J14" s="15">
+      <c r="J14" s="14">
         <v>0</v>
       </c>
-      <c r="K14" s="15">
+      <c r="K14" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
@@ -2862,7 +2864,7 @@
       <c r="G25" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="H25" s="18" t="s">
+      <c r="H25" s="17" t="s">
         <v>108</v>
       </c>
     </row>
@@ -3048,7 +3050,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C26:C30" xr:uid="{9C5F6332-F176-4FA4-AE9F-177D4632FBCB}">
       <formula1>$C$4:$C$8</formula1>
     </dataValidation>
@@ -3115,7 +3117,7 @@
       </c>
     </row>
     <row r="4" spans="2:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="14"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="3" t="s">
         <v>12</v>
       </c>
@@ -3124,7 +3126,7 @@
       </c>
     </row>
     <row r="5" spans="2:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="14"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="3" t="s">
         <v>13</v>
       </c>
@@ -3133,7 +3135,7 @@
       </c>
     </row>
     <row r="6" spans="2:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="14"/>
+      <c r="B6" s="19"/>
       <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
@@ -3142,7 +3144,7 @@
       </c>
     </row>
     <row r="7" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="14"/>
+      <c r="B7" s="19"/>
       <c r="C7" s="3" t="s">
         <v>15</v>
       </c>
@@ -3151,7 +3153,7 @@
       </c>
     </row>
     <row r="8" spans="2:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="14"/>
+      <c r="B8" s="19"/>
       <c r="C8" s="4" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Padronização de acesso ao banco PDO
</commit_message>
<xml_diff>
--- a/_adm/_Cadastros app MYSQL.xlsx
+++ b/_adm/_Cadastros app MYSQL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\securedb\_adm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D718325F-4F8B-40AA-AFF4-8687A07917C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBEA4559-FA30-4070-99F6-99E321A54515}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A00387D4-E64E-4392-9601-70E56E667E9A}"/>
   </bookViews>
@@ -20,7 +20,6 @@
     <sheet name="Viewer" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="122">
   <si>
     <t>Ambientes</t>
   </si>
@@ -387,6 +386,21 @@
   </si>
   <si>
     <t>respname</t>
+  </si>
+  <si>
+    <t>adm_errors</t>
+  </si>
+  <si>
+    <t>from</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>sql</t>
+  </si>
+  <si>
+    <t>dtregister</t>
   </si>
 </sst>
 </file>
@@ -2509,10 +2523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0080EB5-8FF3-4500-94A4-3766A8BA9D9D}">
-  <dimension ref="B3:K39"/>
+  <dimension ref="B3:K43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3047,6 +3061,28 @@
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>83</v>
+      </c>
+      <c r="C43" t="s">
+        <v>118</v>
+      </c>
+      <c r="D43" t="s">
+        <v>120</v>
+      </c>
+      <c r="E43" t="s">
+        <v>119</v>
+      </c>
+      <c r="F43" t="s">
+        <v>121</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
tela login ajustada e permissões de admin e super-user (edicao usuarios)
</commit_message>
<xml_diff>
--- a/_adm/_Cadastros app MYSQL.xlsx
+++ b/_adm/_Cadastros app MYSQL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\securedb\_adm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBEA4559-FA30-4070-99F6-99E321A54515}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C51AA6E0-90E0-47FF-AE26-6FB48B91FF39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A00387D4-E64E-4392-9601-70E56E667E9A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="125">
   <si>
     <t>Ambientes</t>
   </si>
@@ -401,13 +401,22 @@
   </si>
   <si>
     <t>dtregister</t>
+  </si>
+  <si>
+    <t>adm_login_activity</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>ip</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -465,6 +474,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -534,7 +551,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -591,6 +608,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -2523,10 +2541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0080EB5-8FF3-4500-94A4-3766A8BA9D9D}">
-  <dimension ref="B3:K43"/>
+  <dimension ref="B3:K47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3063,7 +3081,7 @@
       <c r="H39" s="1"/>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B42" t="s">
+      <c r="B42" s="20" t="s">
         <v>117</v>
       </c>
     </row>
@@ -3082,6 +3100,28 @@
       </c>
       <c r="F43" t="s">
         <v>121</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B46" s="20" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>121</v>
+      </c>
+      <c r="C47" t="s">
+        <v>123</v>
+      </c>
+      <c r="D47" t="s">
+        <v>84</v>
+      </c>
+      <c r="E47" t="s">
+        <v>124</v>
+      </c>
+      <c r="F47" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CRUD Databases completo e ajustes nas views TABELA (col empresa)...
</commit_message>
<xml_diff>
--- a/_adm/_Cadastros app MYSQL.xlsx
+++ b/_adm/_Cadastros app MYSQL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\securedb\_adm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C51AA6E0-90E0-47FF-AE26-6FB48B91FF39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D920B5ED-4DB5-4EAB-84DC-41FAD3987144}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A00387D4-E64E-4392-9601-70E56E667E9A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="126">
   <si>
     <t>Ambientes</t>
   </si>
@@ -410,13 +410,16 @@
   </si>
   <si>
     <t>ip</t>
+  </si>
+  <si>
+    <t>iddb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -486,6 +489,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -551,7 +561,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -605,16 +615,34 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="93">
+  <dxfs count="94">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2047,198 +2075,199 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{CE6B4342-CBFA-473D-8302-1E748C465A67}" name="Tabela10" displayName="Tabela10" ref="B4:G8" totalsRowShown="0" dataDxfId="92">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{CE6B4342-CBFA-473D-8302-1E748C465A67}" name="Tabela10" displayName="Tabela10" ref="B4:G8" totalsRowShown="0" dataDxfId="93">
   <autoFilter ref="B4:G8" xr:uid="{EA0BA91C-0053-4873-B377-F4C9B118EF81}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{4312BCB8-21CE-427F-88A7-93C626B67CB4}" name="idcia" dataDxfId="91"/>
-    <tableColumn id="2" xr3:uid="{CF3C2B84-D621-45A1-B55F-0A0AA8694AFF}" name="cianame" dataDxfId="90"/>
-    <tableColumn id="5" xr3:uid="{11AC588F-E33E-498E-90C3-DA4FAB1B095C}" name="respname" dataDxfId="89"/>
-    <tableColumn id="6" xr3:uid="{6C76FE8B-145E-4E8B-82FE-4FBA8DBA606A}" name="email" dataDxfId="88"/>
-    <tableColumn id="7" xr3:uid="{BEE80F0E-A884-4CEE-8FED-72BF33FFC95A}" name="celphone" dataDxfId="87"/>
-    <tableColumn id="3" xr3:uid="{BB764F07-0EF8-4779-AAF3-081A310C3134}" name="status" dataDxfId="86"/>
+    <tableColumn id="1" xr3:uid="{4312BCB8-21CE-427F-88A7-93C626B67CB4}" name="idcia" dataDxfId="92"/>
+    <tableColumn id="2" xr3:uid="{CF3C2B84-D621-45A1-B55F-0A0AA8694AFF}" name="cianame" dataDxfId="91"/>
+    <tableColumn id="5" xr3:uid="{11AC588F-E33E-498E-90C3-DA4FAB1B095C}" name="respname" dataDxfId="90"/>
+    <tableColumn id="6" xr3:uid="{6C76FE8B-145E-4E8B-82FE-4FBA8DBA606A}" name="email" dataDxfId="89"/>
+    <tableColumn id="7" xr3:uid="{BEE80F0E-A884-4CEE-8FED-72BF33FFC95A}" name="celphone" dataDxfId="88"/>
+    <tableColumn id="3" xr3:uid="{BB764F07-0EF8-4779-AAF3-081A310C3134}" name="status" dataDxfId="87"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium25" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{117599F9-7BC4-4FFC-A14F-9880FA008D62}" name="Tabela4" displayName="Tabela4" ref="C3:C8" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39" tableBorderDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{117599F9-7BC4-4FFC-A14F-9880FA008D62}" name="Tabela4" displayName="Tabela4" ref="C3:C8" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40" tableBorderDxfId="39">
   <autoFilter ref="C3:C8" xr:uid="{C6E10A1E-B17D-4DA0-A721-41F80C7BCC6E}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{FEFBDF3E-6414-4FDF-8922-F1B23A103788}" name="TNS" dataDxfId="37"/>
+    <tableColumn id="1" xr3:uid="{FEFBDF3E-6414-4FDF-8922-F1B23A103788}" name="TNS" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium24" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{2CB9C6E2-B2BE-4447-A442-E97A818F5177}" name="Tabela414" displayName="Tabela414" ref="F3:F8" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35" tableBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{2CB9C6E2-B2BE-4447-A442-E97A818F5177}" name="Tabela414" displayName="Tabela414" ref="F3:F8" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36" tableBorderDxfId="35">
   <autoFilter ref="F3:F8" xr:uid="{5D526376-D6EB-4486-89BA-AEDFFE8888E9}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{B4A2BFFC-74D7-482D-9CB6-444A21A14746}" name="PROGRAM" dataDxfId="33"/>
+    <tableColumn id="1" xr3:uid="{B4A2BFFC-74D7-482D-9CB6-444A21A14746}" name="PROGRAM" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium25" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{1886F047-E801-4F28-9BAE-1E0CDCFFC04D}" name="Tabela115" displayName="Tabela115" ref="F11:I12" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{1886F047-E801-4F28-9BAE-1E0CDCFFC04D}" name="Tabela115" displayName="Tabela115" ref="F11:I12" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
   <autoFilter ref="F11:I12" xr:uid="{5D25EB8E-91DF-4172-B5F4-E533114D351A}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{17FE0A75-2457-40A1-99E9-0A466CC1D9FB}" name="Data" dataDxfId="30"/>
-    <tableColumn id="2" xr3:uid="{B8DF1968-D98D-42A1-8F9B-8A42BB6F4E26}" name="USERNAME" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{CB4BDD2E-CDB2-4077-B902-9D6D8A357D83}" name="OSUSER" dataDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{1466B965-A111-47F5-8CF6-1B6A0F27002E}" name="MACHINE" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{17FE0A75-2457-40A1-99E9-0A466CC1D9FB}" name="Data" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{B8DF1968-D98D-42A1-8F9B-8A42BB6F4E26}" name="USERNAME" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{CB4BDD2E-CDB2-4077-B902-9D6D8A357D83}" name="OSUSER" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{1466B965-A111-47F5-8CF6-1B6A0F27002E}" name="MACHINE" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium25" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{44884F21-7769-4BD2-909A-1E31250F9095}" name="Tabela510" displayName="Tabela510" ref="B6:G13" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{44884F21-7769-4BD2-909A-1E31250F9095}" name="Tabela510" displayName="Tabela510" ref="B6:G13" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
   <autoFilter ref="B6:G13" xr:uid="{94A45C83-F8A5-4D97-83AD-DA40AE6781D1}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{700AC22E-D27F-4BC7-B7F5-34F1B2137640}" name="QTD" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{A662147F-3BCD-4BDE-AE8D-4149CCCBC801}" name="Username" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{9B37164F-A883-4C40-81DB-B40062874D74}" name="OSUser" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{384C905F-C0E0-4ED0-8095-EEC1CBAB51CA}" name="Machine" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{63466D1C-3057-40D4-93AA-E5F7642EC14D}" name="Program" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{C60D9824-F037-4E66-8F44-2D9C74CC5BCA}" name="Status" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{700AC22E-D27F-4BC7-B7F5-34F1B2137640}" name="QTD" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{A662147F-3BCD-4BDE-AE8D-4149CCCBC801}" name="Username" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{9B37164F-A883-4C40-81DB-B40062874D74}" name="OSUser" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{384C905F-C0E0-4ED0-8095-EEC1CBAB51CA}" name="Machine" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{63466D1C-3057-40D4-93AA-E5F7642EC14D}" name="Program" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{C60D9824-F037-4E66-8F44-2D9C74CC5BCA}" name="Status" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium25" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{0811E8F2-F425-47CB-BCC2-633474B4D7B6}" name="Tabela15" displayName="Tabela15" ref="I6:I7" insertRow="1" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{0811E8F2-F425-47CB-BCC2-633474B4D7B6}" name="Tabela15" displayName="Tabela15" ref="I6:I7" insertRow="1" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="I6:I7" xr:uid="{4F731ABB-2DCB-4CA1-97B4-809D15751A10}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{012C9BAF-DECD-45CC-84B2-0007FDA9CD42}" name="USERNAME" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{012C9BAF-DECD-45CC-84B2-0007FDA9CD42}" name="USERNAME" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium25" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{F2FEDA15-E48A-46B2-ADE2-857CC1107CAA}" name="Tabela541113" displayName="Tabela541113" ref="B5:O12" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{F2FEDA15-E48A-46B2-ADE2-857CC1107CAA}" name="Tabela541113" displayName="Tabela541113" ref="B5:O12" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="B5:O12" xr:uid="{FA9BC69B-F4B4-484A-AE2F-15EEF07BADAB}"/>
   <tableColumns count="14">
-    <tableColumn id="2" xr3:uid="{6949D402-5241-4165-95FE-277FA407A798}" name="Username" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{6D86510B-85D5-4AD8-953B-45A251A095FD}" name="OSUser" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{B43A5AAA-6EC3-4D3D-84FA-A51F98E151B8}" name="Machine" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{443BB74C-6BB5-499E-8C22-EFE1D0453E8B}" name="Dt.Inicio" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{F39BB5B0-A3A8-42D2-96E3-7E96DCA65153}" name="Dt.Fim" dataDxfId="9"/>
-    <tableColumn id="1" xr3:uid="{2E5364E9-E283-4547-9F83-61A8050FD41A}" name="Tools" dataDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{1FA6C5E4-E58E-421F-A761-3C635C7DADE4}" name="Sessões por Usuário" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{2AF58C69-2939-48B7-A278-50800C8AFFE3}" name="LogUser" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{5B1FF714-5F0C-4FAA-9E1C-39B57C01928A}" name="Trace" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{E54A7B0F-B61C-4127-8E4C-73E6B24108AB}" name="Cursor Sharing" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{755A179F-FC51-40ED-9A5F-3F57754D6D3E}" name="INIT PL/SQL" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{981E64EF-623C-44A3-816D-E1D80C5EB0BC}" name="OBS" dataDxfId="2"/>
-    <tableColumn id="13" xr3:uid="{BFC22A29-29BA-476F-AF19-4DB9198B27E7}" name="Grantor Username" dataDxfId="1"/>
-    <tableColumn id="14" xr3:uid="{EE723761-82B5-4C7F-9F41-A78AAD6F6D48}" name="Grantor OSUSER" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{6949D402-5241-4165-95FE-277FA407A798}" name="Username" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{6D86510B-85D5-4AD8-953B-45A251A095FD}" name="OSUser" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{B43A5AAA-6EC3-4D3D-84FA-A51F98E151B8}" name="Machine" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{443BB74C-6BB5-499E-8C22-EFE1D0453E8B}" name="Dt.Inicio" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{F39BB5B0-A3A8-42D2-96E3-7E96DCA65153}" name="Dt.Fim" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{2E5364E9-E283-4547-9F83-61A8050FD41A}" name="Tools" dataDxfId="9"/>
+    <tableColumn id="11" xr3:uid="{1FA6C5E4-E58E-421F-A761-3C635C7DADE4}" name="Sessões por Usuário" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{2AF58C69-2939-48B7-A278-50800C8AFFE3}" name="LogUser" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{5B1FF714-5F0C-4FAA-9E1C-39B57C01928A}" name="Trace" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{E54A7B0F-B61C-4127-8E4C-73E6B24108AB}" name="Cursor Sharing" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{755A179F-FC51-40ED-9A5F-3F57754D6D3E}" name="INIT PL/SQL" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{981E64EF-623C-44A3-816D-E1D80C5EB0BC}" name="OBS" dataDxfId="3"/>
+    <tableColumn id="13" xr3:uid="{BFC22A29-29BA-476F-AF19-4DB9198B27E7}" name="Grantor Username" dataDxfId="2"/>
+    <tableColumn id="14" xr3:uid="{EE723761-82B5-4C7F-9F41-A78AAD6F6D48}" name="Grantor OSUSER" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium25" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{6D809C67-C871-4059-9A1D-F2E218B00897}" name="Tabela11" displayName="Tabela11" ref="B11:K14" totalsRowShown="0" dataDxfId="85">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{6D809C67-C871-4059-9A1D-F2E218B00897}" name="Tabela11" displayName="Tabela11" ref="B11:K14" totalsRowShown="0" dataDxfId="86">
   <autoFilter ref="B11:K14" xr:uid="{5C835B22-5BC8-4F39-A059-93F7A987AFB8}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{9E148F98-1FD3-49C1-A9BB-F1A1805EA7F5}" name="iduser" dataDxfId="84"/>
-    <tableColumn id="2" xr3:uid="{1D7712DB-DB75-4B66-8A5E-0AB98D15D1B0}" name="idcia" dataDxfId="83"/>
-    <tableColumn id="3" xr3:uid="{2FAB6B79-A789-4A77-89F6-BA0C56C86D35}" name="name" dataDxfId="82"/>
+    <tableColumn id="1" xr3:uid="{9E148F98-1FD3-49C1-A9BB-F1A1805EA7F5}" name="iduser" dataDxfId="85"/>
+    <tableColumn id="2" xr3:uid="{1D7712DB-DB75-4B66-8A5E-0AB98D15D1B0}" name="idcia" dataDxfId="84"/>
+    <tableColumn id="3" xr3:uid="{2FAB6B79-A789-4A77-89F6-BA0C56C86D35}" name="name" dataDxfId="83"/>
     <tableColumn id="4" xr3:uid="{62787CAB-A3F2-4E0F-A55D-8680E7A300AD}" name="loginuser"/>
     <tableColumn id="5" xr3:uid="{99633B34-30C0-45B9-83B1-67B8F0C06954}" name="Password"/>
-    <tableColumn id="6" xr3:uid="{233A1894-FA95-49D7-AFDC-C98113F737F1}" name="email" dataDxfId="81" dataCellStyle="Hiperlink"/>
-    <tableColumn id="10" xr3:uid="{A5BF7DD2-C44A-4E80-B5E6-E614834AE381}" name="celphone" dataDxfId="80" dataCellStyle="Hiperlink"/>
-    <tableColumn id="7" xr3:uid="{C5E32CB7-6B92-4324-BB4A-D0D7D06693B4}" name="status" dataDxfId="79"/>
-    <tableColumn id="8" xr3:uid="{B2745FC3-C449-4AA1-B9A0-85D0F3464D19}" name="admin" dataDxfId="78"/>
-    <tableColumn id="9" xr3:uid="{7C9F39C1-8A41-45EA-BF5B-F8748B7872C1}" name="superuser" dataDxfId="77"/>
+    <tableColumn id="6" xr3:uid="{233A1894-FA95-49D7-AFDC-C98113F737F1}" name="email" dataDxfId="82" dataCellStyle="Hiperlink"/>
+    <tableColumn id="10" xr3:uid="{A5BF7DD2-C44A-4E80-B5E6-E614834AE381}" name="celphone" dataDxfId="81" dataCellStyle="Hiperlink"/>
+    <tableColumn id="7" xr3:uid="{C5E32CB7-6B92-4324-BB4A-D0D7D06693B4}" name="status" dataDxfId="80"/>
+    <tableColumn id="8" xr3:uid="{B2745FC3-C449-4AA1-B9A0-85D0F3464D19}" name="admin" dataDxfId="79"/>
+    <tableColumn id="9" xr3:uid="{7C9F39C1-8A41-45EA-BF5B-F8748B7872C1}" name="superuser" dataDxfId="78"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium25" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{12B0385F-B1A1-41AC-814A-6522E4A300D7}" name="Tabela117" displayName="Tabela117" ref="B18:D22" totalsRowShown="0" headerRowDxfId="76" dataDxfId="75">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{12B0385F-B1A1-41AC-814A-6522E4A300D7}" name="Tabela117" displayName="Tabela117" ref="B18:D22" totalsRowShown="0" headerRowDxfId="77" dataDxfId="76">
   <autoFilter ref="B18:D22" xr:uid="{4453047C-8941-416A-9E0E-9E5669C82504}"/>
   <tableColumns count="3">
-    <tableColumn id="3" xr3:uid="{79C72FA5-8DE0-4B65-AD54-38A81CB993FA}" name="idcia" dataDxfId="74"/>
-    <tableColumn id="1" xr3:uid="{09C1CEBC-A44B-455A-84FB-54C83A83CA7C}" name="categor" dataDxfId="73"/>
-    <tableColumn id="2" xr3:uid="{86C5BE9C-C7D4-48D0-93C7-7A4D5E54E773}" name="descat" dataDxfId="72"/>
+    <tableColumn id="3" xr3:uid="{79C72FA5-8DE0-4B65-AD54-38A81CB993FA}" name="idcia" dataDxfId="75"/>
+    <tableColumn id="1" xr3:uid="{09C1CEBC-A44B-455A-84FB-54C83A83CA7C}" name="categor" dataDxfId="74"/>
+    <tableColumn id="2" xr3:uid="{86C5BE9C-C7D4-48D0-93C7-7A4D5E54E773}" name="descat" dataDxfId="73"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium25" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{C8030295-3190-4C6E-82FC-477278DBF0E6}" name="Tabela218" displayName="Tabela218" ref="B25:H30" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70">
-  <autoFilter ref="B25:H30" xr:uid="{74CF12DE-3DF6-45DD-947E-BFE77700D033}"/>
-  <tableColumns count="7">
-    <tableColumn id="3" xr3:uid="{D62E88F7-48BD-48B7-BD7F-F18204103C78}" name="idcia" dataDxfId="69"/>
-    <tableColumn id="1" xr3:uid="{92AF37FD-5952-4276-80C0-6A5E7149F8A2}" name="databasename" dataDxfId="68"/>
-    <tableColumn id="2" xr3:uid="{2D00C2D1-6D76-4C1D-A536-B2C399989BEF}" name="category" dataDxfId="67"/>
-    <tableColumn id="5" xr3:uid="{3F93EB93-4C83-4EB3-8C77-D0AC52CC95AC}" name="host" dataDxfId="66"/>
-    <tableColumn id="6" xr3:uid="{D63EAF68-822E-46F9-A1A5-F62C2B2540C8}" name="dbname" dataDxfId="65"/>
-    <tableColumn id="7" xr3:uid="{61D4C29B-D324-4AA3-8F28-C625977E703B}" name="username" dataDxfId="64"/>
-    <tableColumn id="8" xr3:uid="{FD703B5D-208C-4E3D-B57B-DE9584D70A15}" name="password" dataDxfId="63"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{C8030295-3190-4C6E-82FC-477278DBF0E6}" name="Tabela218" displayName="Tabela218" ref="B25:I30" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71">
+  <autoFilter ref="B25:I30" xr:uid="{74CF12DE-3DF6-45DD-947E-BFE77700D033}"/>
+  <tableColumns count="8">
+    <tableColumn id="4" xr3:uid="{5583D558-2BFD-4946-B99A-70BF08F6A2D1}" name="iddb" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{D62E88F7-48BD-48B7-BD7F-F18204103C78}" name="idcia" dataDxfId="70"/>
+    <tableColumn id="1" xr3:uid="{92AF37FD-5952-4276-80C0-6A5E7149F8A2}" name="databasename" dataDxfId="69"/>
+    <tableColumn id="2" xr3:uid="{2D00C2D1-6D76-4C1D-A536-B2C399989BEF}" name="category" dataDxfId="68"/>
+    <tableColumn id="5" xr3:uid="{3F93EB93-4C83-4EB3-8C77-D0AC52CC95AC}" name="host" dataDxfId="67"/>
+    <tableColumn id="6" xr3:uid="{D63EAF68-822E-46F9-A1A5-F62C2B2540C8}" name="dbname" dataDxfId="66"/>
+    <tableColumn id="7" xr3:uid="{61D4C29B-D324-4AA3-8F28-C625977E703B}" name="username" dataDxfId="65"/>
+    <tableColumn id="8" xr3:uid="{FD703B5D-208C-4E3D-B57B-DE9584D70A15}" name="password" dataDxfId="64"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium25" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{009A29F3-4BFA-40BC-81F7-105CE74E7BED}" name="Tabela419" displayName="Tabela419" ref="B34:B39" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61" tableBorderDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{009A29F3-4BFA-40BC-81F7-105CE74E7BED}" name="Tabela419" displayName="Tabela419" ref="B34:B39" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62" tableBorderDxfId="61">
   <autoFilter ref="B34:B39" xr:uid="{B229024B-3BC2-4C6D-9586-CC75AE5A0472}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{B43FB459-1AD3-4F77-9D76-578795941534}" name="TNS" dataDxfId="59"/>
+    <tableColumn id="1" xr3:uid="{B43FB459-1AD3-4F77-9D76-578795941534}" name="TNS" dataDxfId="60"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium24" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{65CD7931-A024-4F6D-9967-6CF5AABD86F2}" name="Tabela41420" displayName="Tabela41420" ref="C34:C39" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57" tableBorderDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{65CD7931-A024-4F6D-9967-6CF5AABD86F2}" name="Tabela41420" displayName="Tabela41420" ref="C34:C39" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58" tableBorderDxfId="57">
   <autoFilter ref="C34:C39" xr:uid="{E89416BE-A200-4BA3-809B-106F021D56A7}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{ACC89BFB-B9F7-4DB8-A95C-B3FB95412F23}" name="PROGRAM" dataDxfId="55"/>
+    <tableColumn id="1" xr3:uid="{ACC89BFB-B9F7-4DB8-A95C-B3FB95412F23}" name="PROGRAM" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium25" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{8776950F-2CB1-4D74-B675-879D864C7C5A}" name="Tabela11521" displayName="Tabela11521" ref="D34:G35" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{8776950F-2CB1-4D74-B675-879D864C7C5A}" name="Tabela11521" displayName="Tabela11521" ref="D34:G35" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
   <autoFilter ref="D34:G35" xr:uid="{B790A7DD-ED53-4FA8-91ED-16F0C10E4DC1}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{08BA3056-0339-4817-9E3A-B161B0BAE367}" name="Data" dataDxfId="52"/>
-    <tableColumn id="2" xr3:uid="{7A97437C-475E-4C34-B135-DE3B2AD5A7AC}" name="USERNAME" dataDxfId="51"/>
-    <tableColumn id="3" xr3:uid="{332C3A08-2212-40AC-BD5A-B9CE10A33233}" name="OSUSER" dataDxfId="50"/>
-    <tableColumn id="4" xr3:uid="{1C44CCFA-C55A-4A9A-A85D-AB97A44AEFE9}" name="MACHINE" dataDxfId="49"/>
+    <tableColumn id="1" xr3:uid="{08BA3056-0339-4817-9E3A-B161B0BAE367}" name="Data" dataDxfId="53"/>
+    <tableColumn id="2" xr3:uid="{7A97437C-475E-4C34-B135-DE3B2AD5A7AC}" name="USERNAME" dataDxfId="52"/>
+    <tableColumn id="3" xr3:uid="{332C3A08-2212-40AC-BD5A-B9CE10A33233}" name="OSUSER" dataDxfId="51"/>
+    <tableColumn id="4" xr3:uid="{1C44CCFA-C55A-4A9A-A85D-AB97A44AEFE9}" name="MACHINE" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium25" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AE0AF349-CF1A-428A-A441-10B8C64741C7}" name="Tabela1" displayName="Tabela1" ref="C11:D15" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AE0AF349-CF1A-428A-A441-10B8C64741C7}" name="Tabela1" displayName="Tabela1" ref="C11:D15" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
   <autoFilter ref="C11:D15" xr:uid="{FF6AADAE-530D-4CDA-8713-5E777F4D6B64}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{EA1FC018-DD82-49D0-ABC3-079CF18C1AD2}" name="Ambientes" dataDxfId="46"/>
-    <tableColumn id="2" xr3:uid="{F73778B9-D619-4440-81FB-50C8EE9517E0}" name="DESC" dataDxfId="45"/>
+    <tableColumn id="1" xr3:uid="{EA1FC018-DD82-49D0-ABC3-079CF18C1AD2}" name="Ambientes" dataDxfId="47"/>
+    <tableColumn id="2" xr3:uid="{F73778B9-D619-4440-81FB-50C8EE9517E0}" name="DESC" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium25" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{09D064AD-C27E-4B24-9657-A76B6B8A1E9A}" name="Tabela2" displayName="Tabela2" ref="C18:D23" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{09D064AD-C27E-4B24-9657-A76B6B8A1E9A}" name="Tabela2" displayName="Tabela2" ref="C18:D23" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
   <autoFilter ref="C18:D23" xr:uid="{20F04E8A-D3AC-4A3B-A97F-B3624C6D18AA}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{6567C651-5BD0-43EA-A2D0-5ED018FCFC86}" name="Banco" dataDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{EB59A4AE-D691-4B6E-952B-62CDB1B581FC}" name="Ambiente" dataDxfId="41"/>
+    <tableColumn id="1" xr3:uid="{6567C651-5BD0-43EA-A2D0-5ED018FCFC86}" name="Banco" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{EB59A4AE-D691-4B6E-952B-62CDB1B581FC}" name="Ambiente" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium25" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2543,8 +2572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0080EB5-8FF3-4500-94A4-3766A8BA9D9D}">
   <dimension ref="B3:K47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2792,14 +2821,14 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" s="13" t="s">
         <v>104</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="5"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>76</v>
       </c>
@@ -2810,7 +2839,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" s="1">
         <v>1</v>
       </c>
@@ -2821,7 +2850,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20" s="1">
         <v>1</v>
       </c>
@@ -2833,7 +2862,7 @@
       </c>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" s="1">
         <v>1</v>
       </c>
@@ -2845,7 +2874,7 @@
       </c>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22" s="1">
         <v>1</v>
       </c>
@@ -2857,7 +2886,7 @@
       </c>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="5"/>
@@ -2866,7 +2895,7 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B24" s="13" t="s">
         <v>103</v>
       </c>
@@ -2877,109 +2906,127 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="F25" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="G25" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="H25" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="H25" s="17" t="s">
+      <c r="I25" s="17" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="1">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B26" s="21">
         <v>1</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="1">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="G26" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="H26" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="H26" s="1"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B27" s="1">
+        <v>2</v>
+      </c>
+      <c r="C27" s="1">
         <v>1</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B28" s="1">
+        <v>3</v>
+      </c>
+      <c r="C28" s="1">
         <v>1</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B29" s="1">
+        <v>4</v>
+      </c>
+      <c r="C29" s="1">
         <v>1</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B30" s="1">
+        <v>5</v>
+      </c>
+      <c r="C30" s="1">
         <v>1</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B33" s="12" t="s">
@@ -3081,7 +3128,7 @@
       <c r="H39" s="1"/>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B42" s="20" t="s">
+      <c r="B42" s="19" t="s">
         <v>117</v>
       </c>
     </row>
@@ -3103,7 +3150,7 @@
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B46" s="20" t="s">
+      <c r="B46" s="19" t="s">
         <v>122</v>
       </c>
     </row>
@@ -3127,10 +3174,10 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C26:C30" xr:uid="{9C5F6332-F176-4FA4-AE9F-177D4632FBCB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D26:D30" xr:uid="{9C5F6332-F176-4FA4-AE9F-177D4632FBCB}">
       <formula1>$C$4:$C$8</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D26:D30" xr:uid="{290CC105-2088-4F66-AAFA-011A63F01DCF}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E26:E30" xr:uid="{290CC105-2088-4F66-AAFA-011A63F01DCF}">
       <formula1>$C$19:$C$22</formula1>
     </dataValidation>
   </dataValidations>
@@ -3193,7 +3240,7 @@
       </c>
     </row>
     <row r="4" spans="2:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="19"/>
+      <c r="B4" s="20"/>
       <c r="C4" s="3" t="s">
         <v>12</v>
       </c>
@@ -3202,7 +3249,7 @@
       </c>
     </row>
     <row r="5" spans="2:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="19"/>
+      <c r="B5" s="20"/>
       <c r="C5" s="3" t="s">
         <v>13</v>
       </c>
@@ -3211,7 +3258,7 @@
       </c>
     </row>
     <row r="6" spans="2:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="19"/>
+      <c r="B6" s="20"/>
       <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
@@ -3220,7 +3267,7 @@
       </c>
     </row>
     <row r="7" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="19"/>
+      <c r="B7" s="20"/>
       <c r="C7" s="3" t="s">
         <v>15</v>
       </c>
@@ -3229,7 +3276,7 @@
       </c>
     </row>
     <row r="8" spans="2:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="19"/>
+      <c r="B8" s="20"/>
       <c r="C8" s="4" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Atualizações tela bloqueio mostrar log e backup
</commit_message>
<xml_diff>
--- a/_adm/_Cadastros app MYSQL.xlsx
+++ b/_adm/_Cadastros app MYSQL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\securedb\_adm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E32398-D4B6-44CE-BF0B-454D78EE59A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7393B9A8-B555-4FAF-AE48-816370FC3E0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{A00387D4-E64E-4392-9601-70E56E667E9A}"/>
   </bookViews>
@@ -25,18 +25,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="145">
   <si>
     <t>Ambientes</t>
   </si>
@@ -429,16 +423,60 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Horas</t>
+  </si>
+  <si>
+    <t>Taxa</t>
+  </si>
+  <si>
+    <t>Quant</t>
+  </si>
+  <si>
+    <t>Licenças</t>
+  </si>
+  <si>
+    <t>Objeto</t>
+  </si>
+  <si>
+    <t>Mês</t>
+  </si>
+  <si>
+    <t>Ano</t>
+  </si>
+  <si>
+    <t>Opções</t>
+  </si>
+  <si>
+    <t>Com Gestão de Acessos</t>
+  </si>
+  <si>
+    <t>Sem Gestão de Acessos</t>
+  </si>
+  <si>
+    <t>Gestão</t>
+  </si>
+  <si>
+    <t>PROPOSTA SEM GESTÃO</t>
+  </si>
+  <si>
+    <t>PROPOSTA COM GESTÃO</t>
+  </si>
+  <si>
+    <t>Desc Licença</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="[h]:mm:ss;@"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -523,33 +561,62 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="9" tint="-0.249977111117893"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color theme="1"/>
+      <sz val="10"/>
+      <color theme="9"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
     <font>
       <b/>
-      <sz val="8"/>
-      <color theme="1"/>
+      <sz val="10"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="7" tint="0.59999389629810485"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -568,8 +635,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -629,6 +714,118 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -636,7 +833,7 @@
     <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -694,80 +891,170 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="15" fillId="6" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="6" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="17" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="13" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="12" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="12" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="13" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="14" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -3389,7 +3676,7 @@
       </c>
     </row>
     <row r="4" spans="2:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="21"/>
+      <c r="B4" s="56"/>
       <c r="C4" s="3" t="s">
         <v>12</v>
       </c>
@@ -3398,7 +3685,7 @@
       </c>
     </row>
     <row r="5" spans="2:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="21"/>
+      <c r="B5" s="56"/>
       <c r="C5" s="3" t="s">
         <v>13</v>
       </c>
@@ -3407,7 +3694,7 @@
       </c>
     </row>
     <row r="6" spans="2:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="21"/>
+      <c r="B6" s="56"/>
       <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
@@ -3416,7 +3703,7 @@
       </c>
     </row>
     <row r="7" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="21"/>
+      <c r="B7" s="56"/>
       <c r="C7" s="3" t="s">
         <v>15</v>
       </c>
@@ -3425,7 +3712,7 @@
       </c>
     </row>
     <row r="8" spans="2:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="21"/>
+      <c r="B8" s="56"/>
       <c r="C8" s="4" t="s">
         <v>16</v>
       </c>
@@ -4120,424 +4407,447 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{761214DD-BBF0-4DD6-9290-43A42EA0AB42}">
-  <dimension ref="A2:N24"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.88671875" style="22"/>
-    <col min="3" max="3" width="9" style="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.88671875" style="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" style="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="24"/>
-    <col min="7" max="7" width="5.88671875" style="40" bestFit="1" customWidth="1"/>
-    <col min="8" max="14" width="7.5546875" style="40" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.88671875" style="24"/>
+    <col min="1" max="1" width="8.88671875" style="21"/>
+    <col min="2" max="2" width="11.5546875" style="21" customWidth="1"/>
+    <col min="3" max="3" width="10" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="5" customWidth="1"/>
+    <col min="8" max="13" width="8.77734375" style="5" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B2" s="32" t="s">
+    <row r="1" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="22"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+    </row>
+    <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="24"/>
+      <c r="B2" s="72" t="s">
         <v>127</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="E2" s="34" t="s">
+      <c r="E2" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="H2"/>
-      <c r="I2" s="44">
-        <v>0.05</v>
-      </c>
-      <c r="J2" s="44">
-        <v>0.1</v>
-      </c>
-      <c r="K2" s="44">
+      <c r="H2" s="27"/>
+      <c r="I2" s="75">
         <v>0.15</v>
       </c>
-      <c r="L2" s="44">
+      <c r="J2" s="75">
         <v>0.2</v>
       </c>
-      <c r="M2" s="44">
+      <c r="K2" s="75">
         <v>0.25</v>
       </c>
-      <c r="N2" s="44">
+      <c r="L2" s="75">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B3" s="25" t="s">
+      <c r="M2" s="75">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="28">
+      <c r="C3" s="29">
+        <v>50</v>
+      </c>
+      <c r="D3" s="30">
+        <f>IF(C3&gt;0,IF(C3&lt;=50,HLOOKUP(C3,H3:M5,2,TRUE),M4),0)</f>
+        <v>150</v>
+      </c>
+      <c r="E3" s="31">
+        <f>D3*C3</f>
+        <v>7500</v>
+      </c>
+      <c r="G3" s="32" t="s">
+        <v>133</v>
+      </c>
+      <c r="H3" s="32">
+        <v>10</v>
+      </c>
+      <c r="I3" s="32">
+        <v>15</v>
+      </c>
+      <c r="J3" s="32">
+        <v>20</v>
+      </c>
+      <c r="K3" s="32">
+        <v>30</v>
+      </c>
+      <c r="L3" s="32">
+        <v>40</v>
+      </c>
+      <c r="M3" s="32">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B4" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" s="29">
         <v>100</v>
       </c>
-      <c r="D3" s="29">
-        <f>IF(C3&gt;0,IF(C3&lt;=50,HLOOKUP(C3,H3:N4,2,TRUE),N4),0)</f>
-        <v>350</v>
-      </c>
-      <c r="E3" s="30">
-        <f>D3*C3</f>
-        <v>35000</v>
-      </c>
-      <c r="H3" s="41">
-        <v>10</v>
-      </c>
-      <c r="I3" s="41">
-        <v>15</v>
-      </c>
-      <c r="J3" s="41">
-        <v>20</v>
-      </c>
-      <c r="K3" s="41">
-        <v>30</v>
-      </c>
-      <c r="L3" s="41">
-        <v>40</v>
-      </c>
-      <c r="M3" s="41">
-        <v>50</v>
-      </c>
-      <c r="N3" s="41">
+      <c r="D4" s="30">
+        <f>IF(C4&gt;0,IF(C4&lt;=50,HLOOKUP(C4,H3:M5,3,TRUE),M5),0)</f>
         <v>60</v>
       </c>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="25" t="s">
+      <c r="E4" s="31">
+        <f>D4*C4</f>
+        <v>6000</v>
+      </c>
+      <c r="G4" s="70" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="30">
+        <v>250</v>
+      </c>
+      <c r="I4" s="30">
+        <f>$H4-($H4*I$2)</f>
+        <v>212.5</v>
+      </c>
+      <c r="J4" s="30">
+        <f t="shared" ref="J4:M5" si="0">$H4-($H4*J$2)</f>
+        <v>200</v>
+      </c>
+      <c r="K4" s="30">
+        <f t="shared" si="0"/>
+        <v>187.5</v>
+      </c>
+      <c r="L4" s="30">
+        <f t="shared" si="0"/>
+        <v>175</v>
+      </c>
+      <c r="M4" s="30">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B5" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5" s="32"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="35">
+        <f>SUM(E3:E4)</f>
+        <v>13500</v>
+      </c>
+      <c r="G5" s="70" t="s">
         <v>126</v>
       </c>
-      <c r="C4" s="28">
-        <v>200</v>
-      </c>
-      <c r="D4" s="29">
-        <f>IF(C4&gt;0,IF(C4&lt;=50,HLOOKUP(C4,H3:N5,3,TRUE),N5),0)</f>
-        <v>105</v>
-      </c>
-      <c r="E4" s="30">
-        <f>D4*C4</f>
-        <v>21000</v>
-      </c>
-      <c r="G4" s="40" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" s="42">
-        <v>500</v>
-      </c>
-      <c r="I4" s="42">
-        <f>$H$4-($H$4*I2)</f>
-        <v>475</v>
-      </c>
-      <c r="J4" s="42">
-        <f t="shared" ref="J4:N4" si="0">$H$4-($H$4*J2)</f>
-        <v>450</v>
-      </c>
-      <c r="K4" s="42">
+      <c r="H5" s="30">
+        <v>100</v>
+      </c>
+      <c r="I5" s="30">
+        <f>$H5-($H5*I$2)</f>
+        <v>85</v>
+      </c>
+      <c r="J5" s="30">
         <f t="shared" si="0"/>
-        <v>425</v>
-      </c>
-      <c r="L4" s="42">
+        <v>80</v>
+      </c>
+      <c r="K5" s="30">
         <f t="shared" si="0"/>
-        <v>400</v>
-      </c>
-      <c r="M4" s="42">
+        <v>75</v>
+      </c>
+      <c r="L5" s="30">
         <f t="shared" si="0"/>
-        <v>375</v>
-      </c>
-      <c r="N4" s="42">
+        <v>70</v>
+      </c>
+      <c r="M5" s="30">
         <f t="shared" si="0"/>
-        <v>350</v>
-      </c>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B5" s="36" t="s">
-        <v>130</v>
-      </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="38">
-        <f>SUM(E3:E4)</f>
-        <v>56000</v>
-      </c>
-      <c r="G5" s="40" t="s">
-        <v>126</v>
-      </c>
-      <c r="H5" s="42">
-        <v>150</v>
-      </c>
-      <c r="I5" s="42">
-        <f>$H$5-($H$5*I2)</f>
-        <v>142.5</v>
-      </c>
-      <c r="J5" s="42">
-        <f t="shared" ref="J5:N5" si="1">$H$5-($H$5*J2)</f>
-        <v>135</v>
-      </c>
-      <c r="K5" s="42">
-        <f t="shared" si="1"/>
-        <v>127.5</v>
-      </c>
-      <c r="L5" s="42">
-        <f t="shared" si="1"/>
-        <v>120</v>
-      </c>
-      <c r="M5" s="42">
-        <f t="shared" si="1"/>
-        <v>112.5</v>
-      </c>
-      <c r="N5" s="42">
-        <f t="shared" si="1"/>
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B6" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="37">
+      <c r="C6" s="37"/>
+      <c r="D6" s="52">
         <f>E5*C6</f>
         <v>0</v>
       </c>
-      <c r="E6" s="38">
+      <c r="E6" s="35">
         <f>E5-D6</f>
-        <v>56000</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="35"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="43"/>
-      <c r="L8" s="43"/>
-      <c r="M8" s="43"/>
-      <c r="N8" s="43"/>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B9" s="32" t="s">
-        <v>127</v>
-      </c>
-      <c r="C9" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="27" t="s">
-        <v>128</v>
-      </c>
-      <c r="E9" s="34" t="s">
+        <v>13500</v>
+      </c>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="38"/>
+      <c r="L6" s="38"/>
+      <c r="M6" s="38"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E7" s="39"/>
+    </row>
+    <row r="8" spans="1:13" s="2" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="24"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B9" s="72" t="s">
+        <v>135</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="E9" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="H9"/>
-      <c r="I9" s="44">
-        <v>0.15</v>
-      </c>
-      <c r="J9" s="44">
-        <v>0.2</v>
-      </c>
-      <c r="K9" s="44">
-        <v>0.25</v>
-      </c>
-      <c r="L9" s="44">
-        <v>0.3</v>
-      </c>
-      <c r="M9" s="44">
-        <v>0.4</v>
-      </c>
-      <c r="N9" s="44"/>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B10" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="28">
-        <v>10</v>
-      </c>
-      <c r="D10" s="29">
-        <f>IF(C10&gt;0,IF(C10&lt;=50,HLOOKUP(C10,H10:M12,2,TRUE),M11),0)</f>
-        <v>500</v>
-      </c>
-      <c r="E10" s="30">
-        <f>D10*C10</f>
-        <v>5000</v>
-      </c>
-      <c r="H10" s="41">
-        <v>10</v>
-      </c>
-      <c r="I10" s="41">
-        <v>15</v>
-      </c>
-      <c r="J10" s="41">
-        <v>20</v>
-      </c>
-      <c r="K10" s="41">
-        <v>30</v>
-      </c>
-      <c r="L10" s="41">
-        <v>40</v>
-      </c>
-      <c r="M10" s="41">
-        <v>50</v>
-      </c>
-      <c r="N10" s="41"/>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B11" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="C11" s="28">
-        <v>20</v>
-      </c>
-      <c r="D11" s="29">
-        <f>IF(C11&gt;0,IF(C11&lt;=50,HLOOKUP(C11,H10:M12,3,TRUE),M12),0)</f>
-        <v>160</v>
-      </c>
-      <c r="E11" s="30">
+      <c r="H9" s="57" t="s">
+        <v>142</v>
+      </c>
+      <c r="I9" s="58"/>
+      <c r="J9" s="58"/>
+      <c r="K9" s="59"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B10" s="33" t="s">
+        <v>134</v>
+      </c>
+      <c r="C10" s="32">
+        <f>SUM(C3:C4)</f>
+        <v>150</v>
+      </c>
+      <c r="D10" s="34"/>
+      <c r="E10" s="31">
+        <f>$E$5</f>
+        <v>13500</v>
+      </c>
+      <c r="H10" s="40" t="str">
+        <f>$C$3 &amp; " Licenças " &amp;$B$3</f>
+        <v>50 Licenças PROD</v>
+      </c>
+      <c r="I10" s="41"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="42">
+        <f>$E$3</f>
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B11" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="C11" s="71">
+        <f>(C10/20)*22</f>
+        <v>165</v>
+      </c>
+      <c r="D11" s="43">
+        <v>100</v>
+      </c>
+      <c r="E11" s="31">
         <f>D11*C11</f>
-        <v>3200</v>
-      </c>
-      <c r="G11" s="40" t="s">
-        <v>1</v>
-      </c>
-      <c r="H11" s="42">
-        <v>500</v>
-      </c>
-      <c r="I11" s="42">
-        <f>$H11-($H11*I$9)</f>
-        <v>425</v>
-      </c>
-      <c r="J11" s="42">
-        <f t="shared" ref="J11:M12" si="2">$H11-($H11*J$9)</f>
-        <v>400</v>
-      </c>
+        <v>16500</v>
+      </c>
+      <c r="H11" s="44" t="str">
+        <f>$C$4 &amp; " Licenças " &amp;$B$4</f>
+        <v>100 Licenças N-PROD</v>
+      </c>
+      <c r="I11" s="41"/>
+      <c r="J11" s="41"/>
       <c r="K11" s="42">
-        <f t="shared" si="2"/>
-        <v>375</v>
-      </c>
-      <c r="L11" s="42">
-        <f t="shared" si="2"/>
-        <v>350</v>
-      </c>
-      <c r="M11" s="42">
-        <f t="shared" si="2"/>
-        <v>300</v>
-      </c>
-      <c r="N11" s="42"/>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B12" s="36" t="s">
+        <f>$E$4</f>
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="33" t="s">
         <v>130</v>
       </c>
-      <c r="C12" s="26"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="38">
+      <c r="C12" s="32"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="35">
         <f>SUM(E10:E11)</f>
-        <v>8200</v>
-      </c>
-      <c r="G12" s="40" t="s">
-        <v>126</v>
-      </c>
-      <c r="H12" s="42">
+        <v>30000</v>
+      </c>
+      <c r="H12" s="40" t="str">
+        <f>"Desconto " &amp;$C$6*100&amp;"%"</f>
+        <v>Desconto 0%</v>
+      </c>
+      <c r="I12" s="41"/>
+      <c r="J12" s="41"/>
+      <c r="K12" s="45">
+        <f>$D$6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="C13" s="37"/>
+      <c r="D13" s="52">
+        <f>$E$10*$C$13</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="35">
+        <f>E12-D13</f>
+        <v>30000</v>
+      </c>
+      <c r="H13" s="64"/>
+      <c r="I13" s="65"/>
+      <c r="J13" s="65"/>
+      <c r="K13" s="66">
+        <f>K10+K11-K12</f>
+        <v>13500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="F14" s="39"/>
+      <c r="K14" s="48"/>
+    </row>
+    <row r="15" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="F15" s="39"/>
+      <c r="H15" s="60" t="s">
+        <v>143</v>
+      </c>
+      <c r="I15" s="61"/>
+      <c r="J15" s="61"/>
+      <c r="K15" s="62"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B16" s="73" t="s">
+        <v>138</v>
+      </c>
+      <c r="C16" s="74"/>
+      <c r="D16" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="E16" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="F16" s="63"/>
+      <c r="H16" s="49" t="str">
+        <f>$C$3 &amp; " Licenças " &amp;$B$3</f>
+        <v>50 Licenças PROD</v>
+      </c>
+      <c r="I16" s="50"/>
+      <c r="J16" s="50"/>
+      <c r="K16" s="51">
+        <f>$E$3</f>
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B17" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="C17" s="46"/>
+      <c r="D17" s="47">
+        <f>IF($K$13&gt;0,$K$13/$C$10,0)</f>
+        <v>90</v>
+      </c>
+      <c r="E17" s="47">
+        <f>D17*12</f>
+        <v>1080</v>
+      </c>
+      <c r="H17" s="49" t="str">
+        <f>$C$4 &amp; " Licenças " &amp;$B$4</f>
+        <v>100 Licenças N-PROD</v>
+      </c>
+      <c r="I17" s="50"/>
+      <c r="J17" s="50"/>
+      <c r="K17" s="51">
+        <f>$E$4</f>
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B18" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="C18" s="46"/>
+      <c r="D18" s="47">
+        <f>IF($K$21&gt;0,$K$21/$C$10,0)</f>
         <v>200</v>
       </c>
-      <c r="I12" s="42">
-        <f>$H12-($H12*I$9)</f>
-        <v>170</v>
-      </c>
-      <c r="J12" s="42">
-        <f t="shared" si="2"/>
-        <v>160</v>
-      </c>
-      <c r="K12" s="42">
-        <f t="shared" si="2"/>
-        <v>150</v>
-      </c>
-      <c r="L12" s="42">
-        <f t="shared" si="2"/>
-        <v>140</v>
-      </c>
-      <c r="M12" s="42">
-        <f t="shared" si="2"/>
-        <v>120</v>
-      </c>
-      <c r="N12" s="42"/>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B13" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="39">
-        <v>0.15</v>
-      </c>
-      <c r="D13" s="37">
-        <f>E12*C13</f>
-        <v>1230</v>
-      </c>
-      <c r="E13" s="38">
-        <f>E12-D13</f>
-        <v>6970</v>
-      </c>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="E14" s="45"/>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-    </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-    </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-    </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
-    </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-    </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-    </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
+      <c r="E18" s="47">
+        <f>D18*12</f>
+        <v>2400</v>
+      </c>
+      <c r="H18" s="49"/>
+      <c r="I18" s="50"/>
+      <c r="J18" s="50"/>
+      <c r="K18" s="54">
+        <f>K16+K17</f>
+        <v>13500</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C19" s="55"/>
+      <c r="H19" s="49" t="str">
+        <f>"Gestão "&amp;ROUND(C11,0)&amp;" Horas"</f>
+        <v>Gestão 165 Horas</v>
+      </c>
+      <c r="I19" s="50"/>
+      <c r="J19" s="50"/>
+      <c r="K19" s="51">
+        <f>E11</f>
+        <v>16500</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H20" s="49" t="str">
+        <f>"Desconto " &amp;$C$13*100&amp;"%"</f>
+        <v>Desconto 0%</v>
+      </c>
+      <c r="I20" s="50"/>
+      <c r="J20" s="50"/>
+      <c r="K20" s="53">
+        <f>$D$13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H21" s="67"/>
+      <c r="I21" s="68"/>
+      <c r="J21" s="68"/>
+      <c r="K21" s="69">
+        <f>K18+K19-K20</f>
+        <v>30000</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="H15:K15"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>